<commit_message>
add businesses paths into code
</commit_message>
<xml_diff>
--- a/entradas_salida.xlsx
+++ b/entradas_salida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Projects\internship\consolidacion_pw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFED3CE0-1016-45DF-A020-AC7E90A43E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BB3A1E-74EB-4758-8DB1-B938FEF9A99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="19200" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUTAS ENTRADAS Y SALIDA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>entrada</t>
   </si>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B22" sqref="A18:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,9 +480,29 @@
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
@@ -503,13 +523,13 @@
           <x14:formula1>
             <xm:f>_opciones!$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>A4:A1048576</xm:sqref>
+          <xm:sqref>A11:A1048576 A4:A9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F1607AB-0823-4248-9B6B-B1E092AFC664}">
           <x14:formula1>
             <xm:f>_opciones!A3</xm:f>
           </x14:formula1>
-          <xm:sqref>A2</xm:sqref>
+          <xm:sqref>A2 A10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3CDB2C6B-EC5D-4752-B976-2D8B8C98D3EB}">
           <x14:formula1>

</xml_diff>